<commit_message>
ajout du fichier TODO Cheyette
</commit_message>
<xml_diff>
--- a/TODO_Cheyette.xlsx
+++ b/TODO_Cheyette.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>poiunteur vers fonction shift</t>
   </si>
@@ -100,13 +100,50 @@
   </si>
   <si>
     <t>heritage entre MC cheyette et GenericSwap/swaption - enlever evauateLeg() en doublon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATM </t>
+  </si>
+  <si>
+    <t>jouer avec sigma de la vol locale (sigma_r(t)) et observer les niveaux de vol implicite correspondants (sigma_S(t)) - vol de S(t)</t>
+  </si>
+  <si>
+    <t>les autres paramètres étant constants</t>
+  </si>
+  <si>
+    <t>normalement b_barre négatif (pente du smile). Dans le cas gaussien, ok pour b barre proche de 0</t>
+  </si>
+  <si>
+    <t>une fois qu'on a une idée de la vol implicite ATM et qu'on a fixé des paramètres cohérents (pour avoir sigma_imp = 20%), faire varier le strike pour afficher le smile</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3 param : le strike K ATM, la pente b pour le skew </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ voir pour le shift</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1) mettre toutes les sorties dans un unique fichier </t>
+  </si>
+  <si>
+    <t>2) remplir matrices avec prix approximé, prix MC, intervalles de confiance, et erreurs absolue/relative</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +154,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -161,13 +206,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,180 +510,228 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="6">
+        <v>42184</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75">
+      <c r="A2" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75">
+      <c r="A3" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75">
+      <c r="A4" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75">
+      <c r="A5" s="8"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="H1" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="H19" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="2" t="s">
+    <row r="20" spans="1:13">
+      <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="H2" t="s">
+      <c r="B20" s="2"/>
+      <c r="H20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H21" t="s">
         <v>20</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
         <v>1</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
         <v>2</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
-      <c r="A6" t="s">
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
         <v>3</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H24" t="s">
         <v>14</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
-      <c r="A7" t="s">
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
         <v>4</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E25" t="s">
         <v>5</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H25" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
-      <c r="A9" t="s">
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" t="s">
+      <c r="E27" s="1"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" t="s">
         <v>7</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H29" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" t="s">
+    <row r="30" spans="1:13">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
-      <c r="A14" t="s">
+    <row r="32" spans="1:13">
+      <c r="A32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
-      <c r="A16" t="s">
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
         <v>10</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H34" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
         <v>15</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H35" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="s">
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
         <v>11</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E37" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" t="s">
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" t="s">
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="2" t="s">
+    <row r="41" spans="1:8">
+      <c r="A41" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="s">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="5" t="s">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>